<commit_message>
sua lai task của HienNV và chú Vinh
</commit_message>
<xml_diff>
--- a/TaskSheets.xlsx
+++ b/TaskSheets.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CP\group-22-tsmt-svn\trunk\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15348" windowHeight="4656"/>
   </bookViews>
   <sheets>
     <sheet name="Modules" sheetId="3" r:id="rId1"/>
@@ -372,21 +377,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1" tint="4.9989318521683403E-2"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -394,7 +399,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -402,7 +407,7 @@
       <b/>
       <sz val="13"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -706,89 +711,89 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1067,7 +1072,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1075,26 +1080,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.85546875" style="33" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.8984375" style="33" customWidth="1"/>
+    <col min="3" max="3" width="14.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.59765625" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.09765625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>52</v>
       </c>
@@ -1202,7 +1207,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>71</v>
       </c>
@@ -1228,7 +1233,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>71</v>
       </c>
@@ -1246,7 +1251,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
         <v>62</v>
       </c>
@@ -1264,7 +1269,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>62</v>
       </c>
@@ -1282,7 +1287,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>62</v>
       </c>
@@ -1300,7 +1305,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>62</v>
       </c>
@@ -1315,7 +1320,7 @@
       </c>
       <c r="E10" s="29"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>62</v>
       </c>
@@ -1330,7 +1335,7 @@
       </c>
       <c r="E11" s="29"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>62</v>
       </c>
@@ -1403,9 +1408,11 @@
         <v>3</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" s="29"/>
+        <v>55</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
@@ -1452,7 +1459,7 @@
       </c>
       <c r="E19" s="29"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
         <v>63</v>
       </c>
@@ -1467,7 +1474,7 @@
       </c>
       <c r="E20" s="29"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
         <v>69</v>
       </c>
@@ -1484,7 +1491,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
         <v>69</v>
       </c>
@@ -1510,13 +1517,11 @@
         <v>3</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="E23" s="29" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="E23" s="29"/>
+    </row>
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
         <v>65</v>
       </c>
@@ -1533,7 +1538,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
         <v>65</v>
       </c>
@@ -1548,7 +1553,7 @@
       </c>
       <c r="E25" s="29"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
         <v>65</v>
       </c>
@@ -1563,7 +1568,7 @@
       </c>
       <c r="E26" s="29"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
         <v>70</v>
       </c>
@@ -1580,7 +1585,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
         <v>70</v>
       </c>
@@ -1597,7 +1602,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="29" t="s">
         <v>70</v>
       </c>
@@ -1627,7 +1632,7 @@
       </c>
       <c r="E30" s="29"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
         <v>70</v>
       </c>
@@ -1642,7 +1647,7 @@
       </c>
       <c r="E31" s="29"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="29" t="s">
         <v>70</v>
       </c>
@@ -1657,7 +1662,7 @@
       </c>
       <c r="E32" s="29"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="29" t="s">
         <v>70</v>
       </c>
@@ -1672,7 +1677,7 @@
       </c>
       <c r="E33" s="30"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="s">
         <v>67</v>
       </c>
@@ -1688,7 +1693,14 @@
       <c r="E34" s="29"/>
     </row>
   </sheetData>
-  <autoFilter ref="D1:D34"/>
+  <autoFilter ref="D1:D34">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Hien"/>
+        <filter val="Vinh"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:E39">
     <sortCondition ref="A16"/>
   </sortState>
@@ -1725,22 +1737,22 @@
       <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.5703125" style="33" customWidth="1"/>
-    <col min="3" max="3" width="57.140625" style="33" customWidth="1"/>
+    <col min="1" max="1" width="16.8984375" style="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.59765625" style="33" customWidth="1"/>
+    <col min="3" max="3" width="57.09765625" style="33" customWidth="1"/>
     <col min="4" max="4" width="16" style="42" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="29" customWidth="1"/>
+    <col min="5" max="5" width="16.3984375" style="29" customWidth="1"/>
     <col min="6" max="6" width="16" style="29" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.3984375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.3984375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="2" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
         <v>52</v>
       </c>
@@ -2097,12 +2109,12 @@
       <selection activeCell="N10" sqref="N9:N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.8984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35.09765625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.09765625" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2112,11 +2124,11 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="44"/>
-      <c r="B2" s="45" t="s">
+      <c r="A2" s="71"/>
+      <c r="B2" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="68" t="s">
         <v>47</v>
       </c>
       <c r="D2" s="15" t="s">
@@ -2130,9 +2142,9 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="44"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="52"/>
+      <c r="A3" s="71"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="68"/>
       <c r="D3" s="15" t="s">
         <v>2</v>
       </c>
@@ -2144,9 +2156,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="52"/>
+      <c r="A4" s="71"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="68"/>
       <c r="D4" s="15" t="s">
         <v>3</v>
       </c>
@@ -2156,9 +2168,9 @@
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="44"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="52" t="s">
+      <c r="A5" s="71"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="68" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="15" t="s">
@@ -2172,9 +2184,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="52"/>
+      <c r="A6" s="71"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="68"/>
       <c r="D6" s="15" t="s">
         <v>1</v>
       </c>
@@ -2186,9 +2198,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
-      <c r="B7" s="45"/>
-      <c r="C7" s="52"/>
+      <c r="A7" s="71"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="68"/>
       <c r="D7" s="15" t="s">
         <v>2</v>
       </c>
@@ -2200,9 +2212,9 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="52"/>
+      <c r="A8" s="71"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="68"/>
       <c r="D8" s="15" t="s">
         <v>3</v>
       </c>
@@ -2212,9 +2224,9 @@
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="52" t="s">
+      <c r="A9" s="71"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="68" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="15" t="s">
@@ -2228,9 +2240,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="52"/>
+      <c r="A10" s="71"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="68"/>
       <c r="D10" s="15" t="s">
         <v>1</v>
       </c>
@@ -2242,9 +2254,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
-      <c r="B11" s="45"/>
-      <c r="C11" s="52"/>
+      <c r="A11" s="71"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="68"/>
       <c r="D11" s="15" t="s">
         <v>2</v>
       </c>
@@ -2256,9 +2268,9 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="52"/>
+      <c r="A12" s="71"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="68"/>
       <c r="D12" s="15" t="s">
         <v>3</v>
       </c>
@@ -2268,9 +2280,9 @@
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
-      <c r="B13" s="45"/>
-      <c r="C13" s="52" t="s">
+      <c r="A13" s="71"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="68" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="15" t="s">
@@ -2284,9 +2296,9 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="52"/>
+      <c r="A14" s="71"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="68"/>
       <c r="D14" s="15" t="s">
         <v>1</v>
       </c>
@@ -2298,9 +2310,9 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
-      <c r="B15" s="45"/>
-      <c r="C15" s="52"/>
+      <c r="A15" s="71"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="68"/>
       <c r="D15" s="15" t="s">
         <v>2</v>
       </c>
@@ -2312,9 +2324,9 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="44"/>
-      <c r="B16" s="45"/>
-      <c r="C16" s="52"/>
+      <c r="A16" s="71"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="68"/>
       <c r="D16" s="15" t="s">
         <v>3</v>
       </c>
@@ -2324,21 +2336,21 @@
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="44"/>
-      <c r="B17" s="45"/>
-      <c r="C17" s="53" t="s">
+      <c r="A17" s="71"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="53"/>
+      <c r="D17" s="69"/>
       <c r="E17" s="2">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="44">
+      <c r="A18" s="71">
         <v>2</v>
       </c>
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="46" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="16" t="s">
@@ -2350,8 +2362,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
-      <c r="B19" s="60"/>
+      <c r="A19" s="71"/>
+      <c r="B19" s="47"/>
       <c r="C19" s="16" t="s">
         <v>9</v>
       </c>
@@ -2364,8 +2376,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
-      <c r="B20" s="60"/>
+      <c r="A20" s="71"/>
+      <c r="B20" s="47"/>
       <c r="C20" s="16" t="s">
         <v>10</v>
       </c>
@@ -2375,8 +2387,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="44"/>
-      <c r="B21" s="60"/>
+      <c r="A21" s="71"/>
+      <c r="B21" s="47"/>
       <c r="C21" s="16" t="s">
         <v>11</v>
       </c>
@@ -2389,8 +2401,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
-      <c r="B22" s="60"/>
+      <c r="A22" s="71"/>
+      <c r="B22" s="47"/>
       <c r="C22" s="16" t="s">
         <v>12</v>
       </c>
@@ -2400,8 +2412,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
-      <c r="B23" s="60"/>
+      <c r="A23" s="71"/>
+      <c r="B23" s="47"/>
       <c r="C23" s="17" t="s">
         <v>13</v>
       </c>
@@ -2411,8 +2423,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
-      <c r="B24" s="60"/>
+      <c r="A24" s="71"/>
+      <c r="B24" s="47"/>
       <c r="C24" s="17" t="s">
         <v>27</v>
       </c>
@@ -2425,24 +2437,24 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
-      <c r="B25" s="61"/>
-      <c r="C25" s="70" t="s">
+      <c r="A25" s="71"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="71"/>
+      <c r="D25" s="60"/>
       <c r="E25" s="2">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="44">
+      <c r="A26" s="71">
         <v>6</v>
       </c>
-      <c r="B26" s="54" t="s">
+      <c r="B26" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="54" t="s">
+      <c r="C26" s="51" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="19" t="s">
@@ -2456,9 +2468,9 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="44"/>
-      <c r="B27" s="55"/>
-      <c r="C27" s="55"/>
+      <c r="A27" s="71"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="52"/>
       <c r="D27" s="19" t="s">
         <v>16</v>
       </c>
@@ -2470,9 +2482,9 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
-      <c r="B28" s="55"/>
-      <c r="C28" s="56"/>
+      <c r="A28" s="71"/>
+      <c r="B28" s="52"/>
+      <c r="C28" s="70"/>
       <c r="D28" s="19" t="s">
         <v>17</v>
       </c>
@@ -2482,8 +2494,8 @@
       <c r="F28" s="3"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
-      <c r="B29" s="55"/>
+      <c r="A29" s="71"/>
+      <c r="B29" s="52"/>
       <c r="C29" s="20" t="s">
         <v>18</v>
       </c>
@@ -2493,12 +2505,12 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
-      <c r="B30" s="55"/>
-      <c r="C30" s="68" t="s">
+      <c r="A30" s="71"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="69"/>
+      <c r="D30" s="58"/>
       <c r="E30" s="2">
         <v>29</v>
       </c>
@@ -2507,13 +2519,13 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="44">
+      <c r="A31" s="71">
         <v>4</v>
       </c>
-      <c r="B31" s="62" t="s">
+      <c r="B31" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="49" t="s">
+      <c r="C31" s="65" t="s">
         <v>19</v>
       </c>
       <c r="D31" s="5" t="s">
@@ -2527,9 +2539,9 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="44"/>
-      <c r="B32" s="62"/>
-      <c r="C32" s="49"/>
+      <c r="A32" s="71"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="65"/>
       <c r="D32" s="5" t="s">
         <v>2</v>
       </c>
@@ -2541,9 +2553,9 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="44"/>
-      <c r="B33" s="62"/>
-      <c r="C33" s="49"/>
+      <c r="A33" s="71"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="65"/>
       <c r="D33" s="5" t="s">
         <v>3</v>
       </c>
@@ -2553,9 +2565,9 @@
       <c r="F33" s="3"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="44"/>
-      <c r="B34" s="62"/>
-      <c r="C34" s="49" t="s">
+      <c r="A34" s="71"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="65" t="s">
         <v>20</v>
       </c>
       <c r="D34" s="5" t="s">
@@ -2569,9 +2581,9 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="44"/>
-      <c r="B35" s="62"/>
-      <c r="C35" s="49"/>
+      <c r="A35" s="71"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="65"/>
       <c r="D35" s="5" t="s">
         <v>16</v>
       </c>
@@ -2583,9 +2595,9 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="44"/>
-      <c r="B36" s="62"/>
-      <c r="C36" s="49"/>
+      <c r="A36" s="71"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="65"/>
       <c r="D36" s="5" t="s">
         <v>17</v>
       </c>
@@ -2595,9 +2607,9 @@
       <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="44"/>
-      <c r="B37" s="62"/>
-      <c r="C37" s="49" t="s">
+      <c r="A37" s="71"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="65" t="s">
         <v>22</v>
       </c>
       <c r="D37" s="5" t="s">
@@ -2611,9 +2623,9 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="44"/>
-      <c r="B38" s="62"/>
-      <c r="C38" s="49"/>
+      <c r="A38" s="71"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="65"/>
       <c r="D38" s="5" t="s">
         <v>1</v>
       </c>
@@ -2625,9 +2637,9 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="44"/>
-      <c r="B39" s="62"/>
-      <c r="C39" s="49"/>
+      <c r="A39" s="71"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="65"/>
       <c r="D39" s="5" t="s">
         <v>2</v>
       </c>
@@ -2639,9 +2651,9 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="44"/>
-      <c r="B40" s="62"/>
-      <c r="C40" s="49"/>
+      <c r="A40" s="71"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="65"/>
       <c r="D40" s="5" t="s">
         <v>3</v>
       </c>
@@ -2651,9 +2663,9 @@
       <c r="F40" s="3"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="44"/>
-      <c r="B41" s="62"/>
-      <c r="C41" s="49" t="s">
+      <c r="A41" s="71"/>
+      <c r="B41" s="49"/>
+      <c r="C41" s="65" t="s">
         <v>23</v>
       </c>
       <c r="D41" s="5" t="s">
@@ -2667,9 +2679,9 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="44"/>
-      <c r="B42" s="62"/>
-      <c r="C42" s="49"/>
+      <c r="A42" s="71"/>
+      <c r="B42" s="49"/>
+      <c r="C42" s="65"/>
       <c r="D42" s="5" t="s">
         <v>1</v>
       </c>
@@ -2681,9 +2693,9 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="44"/>
-      <c r="B43" s="62"/>
-      <c r="C43" s="49"/>
+      <c r="A43" s="71"/>
+      <c r="B43" s="49"/>
+      <c r="C43" s="65"/>
       <c r="D43" s="5" t="s">
         <v>2</v>
       </c>
@@ -2695,9 +2707,9 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="44"/>
-      <c r="B44" s="62"/>
-      <c r="C44" s="49"/>
+      <c r="A44" s="71"/>
+      <c r="B44" s="49"/>
+      <c r="C44" s="65"/>
       <c r="D44" s="5" t="s">
         <v>3</v>
       </c>
@@ -2707,8 +2719,8 @@
       <c r="F44" s="3"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="44"/>
-      <c r="B45" s="62"/>
+      <c r="A45" s="71"/>
+      <c r="B45" s="49"/>
       <c r="C45" s="6" t="s">
         <v>24</v>
       </c>
@@ -2718,8 +2730,8 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="44"/>
-      <c r="B46" s="63"/>
+      <c r="A46" s="71"/>
+      <c r="B46" s="50"/>
       <c r="C46" s="6" t="s">
         <v>25</v>
       </c>
@@ -2744,16 +2756,16 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="44">
-        <v>3</v>
-      </c>
-      <c r="B48" s="46" t="s">
+      <c r="A48" s="71">
+        <v>3</v>
+      </c>
+      <c r="B48" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="C48" s="64" t="s">
+      <c r="C48" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="D48" s="65"/>
+      <c r="D48" s="54"/>
       <c r="E48" s="2">
         <v>47</v>
       </c>
@@ -2762,12 +2774,12 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="44"/>
-      <c r="B49" s="46"/>
-      <c r="C49" s="64" t="s">
+      <c r="A49" s="71"/>
+      <c r="B49" s="62"/>
+      <c r="C49" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="D49" s="65"/>
+      <c r="D49" s="54"/>
       <c r="E49" s="2">
         <v>48</v>
       </c>
@@ -2776,34 +2788,34 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="44"/>
-      <c r="B50" s="46"/>
-      <c r="C50" s="64" t="s">
+      <c r="A50" s="71"/>
+      <c r="B50" s="62"/>
+      <c r="C50" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="D50" s="65"/>
+      <c r="D50" s="54"/>
       <c r="E50" s="2">
         <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="44"/>
-      <c r="B51" s="46"/>
-      <c r="C51" s="64" t="s">
+      <c r="A51" s="71"/>
+      <c r="B51" s="62"/>
+      <c r="C51" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D51" s="65"/>
+      <c r="D51" s="54"/>
       <c r="E51" s="2">
         <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="44"/>
-      <c r="B52" s="46"/>
-      <c r="C52" s="64" t="s">
+      <c r="A52" s="71"/>
+      <c r="B52" s="62"/>
+      <c r="C52" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="D52" s="65"/>
+      <c r="D52" s="54"/>
       <c r="E52" s="2">
         <v>51</v>
       </c>
@@ -2824,13 +2836,13 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="44">
+      <c r="A54" s="71">
         <v>5</v>
       </c>
-      <c r="B54" s="47" t="s">
+      <c r="B54" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="C54" s="50" t="s">
+      <c r="C54" s="66" t="s">
         <v>35</v>
       </c>
       <c r="D54" s="13" t="s">
@@ -2842,9 +2854,9 @@
       <c r="F54" s="3"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="44"/>
-      <c r="B55" s="47"/>
-      <c r="C55" s="50"/>
+      <c r="A55" s="71"/>
+      <c r="B55" s="63"/>
+      <c r="C55" s="66"/>
       <c r="D55" s="13" t="s">
         <v>37</v>
       </c>
@@ -2856,9 +2868,9 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="44"/>
-      <c r="B56" s="47"/>
-      <c r="C56" s="50"/>
+      <c r="A56" s="71"/>
+      <c r="B56" s="63"/>
+      <c r="C56" s="66"/>
       <c r="D56" s="13" t="s">
         <v>38</v>
       </c>
@@ -2870,9 +2882,9 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="44"/>
-      <c r="B57" s="47"/>
-      <c r="C57" s="50"/>
+      <c r="A57" s="71"/>
+      <c r="B57" s="63"/>
+      <c r="C57" s="66"/>
       <c r="D57" s="13" t="s">
         <v>39</v>
       </c>
@@ -2882,12 +2894,12 @@
       <c r="F57" s="3"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="44"/>
-      <c r="B58" s="47"/>
-      <c r="C58" s="66" t="s">
+      <c r="A58" s="71"/>
+      <c r="B58" s="63"/>
+      <c r="C58" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="D58" s="67"/>
+      <c r="D58" s="56"/>
       <c r="E58" s="2">
         <v>57</v>
       </c>
@@ -2896,12 +2908,12 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="44"/>
-      <c r="B59" s="47"/>
-      <c r="C59" s="66" t="s">
+      <c r="A59" s="71"/>
+      <c r="B59" s="63"/>
+      <c r="C59" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="D59" s="67"/>
+      <c r="D59" s="56"/>
       <c r="E59" s="2">
         <v>58</v>
       </c>
@@ -2910,13 +2922,13 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="44">
+      <c r="A60" s="71">
         <v>7</v>
       </c>
-      <c r="B60" s="48" t="s">
+      <c r="B60" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="C60" s="51" t="s">
+      <c r="C60" s="67" t="s">
         <v>5</v>
       </c>
       <c r="D60" s="14" t="s">
@@ -2930,9 +2942,9 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="44"/>
-      <c r="B61" s="48"/>
-      <c r="C61" s="51"/>
+      <c r="A61" s="71"/>
+      <c r="B61" s="64"/>
+      <c r="C61" s="67"/>
       <c r="D61" s="14" t="s">
         <v>1</v>
       </c>
@@ -2944,9 +2956,9 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="44"/>
-      <c r="B62" s="48"/>
-      <c r="C62" s="51"/>
+      <c r="A62" s="71"/>
+      <c r="B62" s="64"/>
+      <c r="C62" s="67"/>
       <c r="D62" s="14" t="s">
         <v>2</v>
       </c>
@@ -2958,9 +2970,9 @@
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="44"/>
-      <c r="B63" s="48"/>
-      <c r="C63" s="51"/>
+      <c r="A63" s="71"/>
+      <c r="B63" s="64"/>
+      <c r="C63" s="67"/>
       <c r="D63" s="14" t="s">
         <v>3</v>
       </c>
@@ -2970,23 +2982,23 @@
       <c r="F63" s="3"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="44"/>
-      <c r="B64" s="48"/>
-      <c r="C64" s="57" t="s">
+      <c r="A64" s="71"/>
+      <c r="B64" s="64"/>
+      <c r="C64" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="D64" s="58"/>
+      <c r="D64" s="45"/>
       <c r="E64" s="2">
         <v>63</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="44"/>
-      <c r="B65" s="48"/>
-      <c r="C65" s="57" t="s">
+      <c r="A65" s="71"/>
+      <c r="B65" s="64"/>
+      <c r="C65" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="D65" s="58"/>
+      <c r="D65" s="45"/>
       <c r="E65" s="2">
         <v>64</v>
       </c>
@@ -3045,20 +3057,13 @@
   </sheetData>
   <autoFilter ref="F1:F82"/>
   <mergeCells count="37">
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="B18:B25"/>
-    <mergeCell ref="B31:B46"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="A54:A59"/>
+    <mergeCell ref="A60:A65"/>
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="A31:A46"/>
+    <mergeCell ref="A48:A52"/>
     <mergeCell ref="B2:B17"/>
     <mergeCell ref="B48:B52"/>
     <mergeCell ref="B54:B59"/>
@@ -3075,13 +3080,20 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C31:C33"/>
     <mergeCell ref="C26:C28"/>
-    <mergeCell ref="A54:A59"/>
-    <mergeCell ref="A60:A65"/>
-    <mergeCell ref="A2:A17"/>
-    <mergeCell ref="A18:A25"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="A31:A46"/>
-    <mergeCell ref="A48:A52"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="B18:B25"/>
+    <mergeCell ref="B31:B46"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C25:D25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
@@ -3099,7 +3111,7 @@
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>